<commit_message>
Actualizacion en Planificacion - Revision 4 de Octubre d 2011
</commit_message>
<xml_diff>
--- a/Docs/02-Planificacion/WPR/16082011/Status_18082011.xlsx
+++ b/Docs/02-Planificacion/WPR/16082011/Status_18082011.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Sprint</t>
   </si>
@@ -112,6 +112,24 @@
   </si>
   <si>
     <t>Gestion de Planificacion Part 1</t>
+  </si>
+  <si>
+    <t>Gestion de Planificacion Part 2</t>
+  </si>
+  <si>
+    <t>Manual de Usuario y Procedimientos</t>
+  </si>
+  <si>
+    <t>Modulo de Encuestas</t>
+  </si>
+  <si>
+    <t>Modulo de Foro</t>
+  </si>
+  <si>
+    <t>Ciclo de Test de Regresion Completa</t>
+  </si>
+  <si>
+    <t>Bug Fixing</t>
   </si>
 </sst>
 </file>
@@ -190,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +281,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -317,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -342,21 +366,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -366,25 +375,16 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -392,9 +392,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,69 +735,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B1:K10"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A1:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" style="35" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" style="35" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="26"/>
+    <col min="1" max="1" width="6.5703125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="27" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" style="27" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="20" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="20"/>
     <col min="6" max="6" width="14.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.42578125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="30" customWidth="1"/>
-    <col min="11" max="11" width="13" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="17" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="23" customWidth="1"/>
+    <col min="11" max="11" width="13" style="23" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="39.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="23" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="18"/>
-      <c r="J1" s="27" t="s">
+      <c r="I1" s="32"/>
+      <c r="J1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="27"/>
-      <c r="L1" s="16" t="s">
+      <c r="K1" s="33"/>
+      <c r="L1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="32" t="s">
+      <c r="A2" s="35"/>
+      <c r="B2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="18" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="13" t="s">
@@ -780,16 +806,16 @@
       <c r="G2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="21" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="4" t="s">
@@ -803,21 +829,21 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="36">
         <v>1</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="28" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="28">
+      <c r="K3" s="21">
         <v>9</v>
       </c>
       <c r="L3" s="7"/>
@@ -825,27 +851,27 @@
       <c r="N3" s="3"/>
     </row>
     <row r="4" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
+      <c r="A4" s="36">
         <v>2</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="13" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="13">
         <v>2</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="19">
+      <c r="I4" s="14">
         <v>10</v>
       </c>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
       <c r="L4" s="7"/>
       <c r="M4" s="3"/>
       <c r="N4" s="9" t="s">
@@ -853,21 +879,21 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="14">
         <v>8</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
       <c r="L5" s="7"/>
       <c r="M5" s="3"/>
       <c r="N5" s="10" t="s">
@@ -875,35 +901,35 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
-      <c r="H6" s="19" t="s">
+      <c r="H6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="19">
+      <c r="I6" s="14">
         <v>1</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
       <c r="L6" s="7"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="114" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
+      <c r="A7" s="36">
         <v>3</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="18">
         <v>1</v>
       </c>
       <c r="F7" s="13" t="s">
@@ -912,14 +938,14 @@
       <c r="G7" s="13">
         <v>8</v>
       </c>
-      <c r="H7" s="19" t="s">
+      <c r="H7" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="15">
         <v>3</v>
       </c>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
       <c r="L7" s="7"/>
       <c r="M7" s="3"/>
       <c r="N7" s="11" t="s">
@@ -927,13 +953,13 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="57" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="24" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="18">
         <v>8</v>
       </c>
       <c r="F8" s="13" t="s">
@@ -942,10 +968,10 @@
       <c r="G8" s="13">
         <v>5</v>
       </c>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
       <c r="L8" s="7"/>
       <c r="M8" s="3"/>
       <c r="N8" s="11" t="s">
@@ -953,23 +979,23 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14">
+      <c r="A9" s="36">
         <v>4</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="24">
         <v>18</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
       <c r="L9" s="7"/>
       <c r="M9" s="3"/>
       <c r="N9" s="11" t="s">
@@ -977,73 +1003,85 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="32" t="s">
+      <c r="A10" s="36"/>
+      <c r="B10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="32">
-        <v>17</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="C10" s="24">
+        <v>5</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
       <c r="L10" s="7"/>
       <c r="M10" s="3"/>
       <c r="N10" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
+    <row r="11" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="36">
+        <v>5</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="24">
+        <v>11</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
       <c r="L11" s="7"/>
       <c r="M11" s="3"/>
       <c r="N11" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
+    <row r="12" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
       <c r="L12" s="7"/>
       <c r="M12" s="3"/>
       <c r="N12" s="11"/>
     </row>
-    <row r="13" spans="1:14" ht="57" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
+    <row r="13" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36">
+        <v>6</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
       <c r="L13" s="7"/>
       <c r="M13" s="3"/>
       <c r="N13" s="11" t="s">
@@ -1051,33 +1089,41 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="A14" s="37">
+        <v>7</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="26"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="7"/>
       <c r="M14" s="3"/>
       <c r="N14" s="10"/>
     </row>
     <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="A15" s="37">
+        <v>8</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="7"/>
       <c r="M15" s="3"/>
       <c r="N15" s="12" t="s">
@@ -1085,18 +1131,18 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="57" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
-        <v>2</v>
-      </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="7"/>
       <c r="M16" s="3"/>
       <c r="N16" s="11" t="s">
@@ -1104,16 +1150,16 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="57" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
+      <c r="A17" s="37"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
       <c r="L17" s="7"/>
       <c r="M17" s="3"/>
       <c r="N17" s="11" t="s">
@@ -1121,19 +1167,19 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="37">
         <v>3</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
       <c r="L18" s="7"/>
       <c r="M18" s="3"/>
       <c r="N18" s="11" t="s">
@@ -1141,483 +1187,483 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="37">
         <v>4</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
       <c r="L19" s="7"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
       <c r="L20" s="7"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="A21" s="37"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="7"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
+      <c r="A22" s="37"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="7"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="A23" s="37"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
       <c r="L23" s="7"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="A24" s="37"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
       <c r="L24" s="7"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
       <c r="L25" s="7"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
+      <c r="A26" s="37"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
       <c r="L26" s="7"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
+      <c r="A27" s="37"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
       <c r="F27" s="8"/>
       <c r="G27" s="8"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
       <c r="L27" s="7"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
       <c r="L28" s="7"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="22"/>
       <c r="L29" s="7"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
       <c r="L30" s="7"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
+      <c r="A31" s="37"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
       <c r="F31" s="8"/>
       <c r="G31" s="8"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
       <c r="L31" s="7"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="8"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
       <c r="L32" s="7"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
+      <c r="A33" s="37"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
       <c r="L33" s="7"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+      <c r="A34" s="37"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
       <c r="F34" s="8"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
       <c r="L34" s="7"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
+      <c r="A35" s="37"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
       <c r="F35" s="8"/>
       <c r="G35" s="8"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
       <c r="L35" s="7"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
+      <c r="A36" s="37"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
       <c r="L36" s="7"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
+      <c r="A37" s="37"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="29"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
       <c r="L37" s="7"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
+      <c r="A38" s="37"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
       <c r="L38" s="7"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
+      <c r="A39" s="37"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="29"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
       <c r="L39" s="7"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
+      <c r="A40" s="37"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="29"/>
-      <c r="K40" s="29"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="22"/>
       <c r="L40" s="7"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
+      <c r="A41" s="37"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="29"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="16"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="22"/>
       <c r="L41" s="7"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
+      <c r="A42" s="37"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
+      <c r="H42" s="16"/>
+      <c r="I42" s="16"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
       <c r="L42" s="7"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
+      <c r="A43" s="37"/>
+      <c r="B43" s="26"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="29"/>
-      <c r="K43" s="29"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
       <c r="L43" s="7"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
       <c r="L44" s="7"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
+      <c r="A45" s="37"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="29"/>
-      <c r="K45" s="29"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
       <c r="L45" s="7"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
+      <c r="H46" s="16"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="22"/>
       <c r="L46" s="7"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="26"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
       <c r="F47" s="8"/>
       <c r="G47" s="8"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
       <c r="L47" s="7"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
       <c r="F48" s="8"/>
       <c r="G48" s="8"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
       <c r="L48" s="7"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>

</xml_diff>